<commit_message>
adjust something in decision trê
</commit_message>
<xml_diff>
--- a/lophoc.xlsx
+++ b/lophoc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb3917c18517e79c/CNTT/ptdl1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{7E680739-8B6C-4A05-921C-AE2C8798FE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C980B873-5462-48EE-A68C-E0C5486AB429}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{7E680739-8B6C-4A05-921C-AE2C8798FE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE168B63-AA56-4FB3-9295-B7D90F0A51E5}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="2715" windowWidth="12390" windowHeight="9570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -57,12 +57,6 @@
     <t>nắng</t>
   </si>
   <si>
-    <t>có</t>
-  </si>
-  <si>
-    <t>không</t>
-  </si>
-  <si>
     <t>Sức khỏe</t>
   </si>
   <si>
@@ -85,6 +79,12 @@
   </si>
   <si>
     <t>IG thời tiết</t>
+  </si>
+  <si>
+    <t>nghỉ</t>
+  </si>
+  <si>
+    <t>học</t>
   </si>
 </sst>
 </file>
@@ -137,6 +137,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -404,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,7 +421,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -434,7 +438,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -445,7 +449,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -456,7 +460,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -467,40 +471,40 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -512,7 +516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8505B718-8956-4B3B-9537-A013CE8781F2}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -520,7 +524,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1">
         <v>0.99</v>
@@ -528,7 +532,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>0.86</v>
@@ -536,7 +540,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <f xml:space="preserve"> 0.99 - 0.86</f>
@@ -545,7 +549,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>0.99</v>
@@ -553,7 +557,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>0.96</v>
@@ -561,7 +565,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <f>0.99-0.96</f>

</xml_diff>